<commit_message>
Sorting by Field hopefully ready
</commit_message>
<xml_diff>
--- a/data/dataExport.xlsx
+++ b/data/dataExport.xlsx
@@ -18,37 +18,49 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Wiek</t>
+    <t>Data przyjęcia</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>382</t>
+  </si>
+  <si>
+    <t>383</t>
+  </si>
+  <si>
+    <t>384</t>
+  </si>
+  <si>
+    <t>385</t>
   </si>
   <si>
     <t>376</t>
@@ -67,25 +79,15 @@
   </si>
   <si>
     <t>381</t>
-  </si>
-  <si>
-    <t>382</t>
-  </si>
-  <si>
-    <t>383</t>
-  </si>
-  <si>
-    <t>384</t>
-  </si>
-  <si>
-    <t>385</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -115,8 +117,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -142,80 +164,80 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>65.0</v>
+      <c r="B3" s="1" t="n">
+        <v>42696.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>65.0</v>
+      <c r="B4" s="2" t="n">
+        <v>42697.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>57.0</v>
+      <c r="B5" s="3" t="n">
+        <v>42699.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>67.0</v>
+      <c r="B6" s="4" t="n">
+        <v>42704.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
-        <v>68.0</v>
+      <c r="B7" s="5" t="n">
+        <v>42705.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>66.0</v>
+      <c r="B8" s="6" t="n">
+        <v>42708.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>75.0</v>
+      <c r="B9" s="7" t="n">
+        <v>42709.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>69.0</v>
+      <c r="B10" s="8" t="n">
+        <v>42710.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>65.0</v>
+      <c r="B11" s="9" t="n">
+        <v>42711.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>71.0</v>
+      <c r="B12" s="10" t="n">
+        <v>42715.0</v>
       </c>
     </row>
   </sheetData>
@@ -244,80 +266,80 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="n">
-        <v>77.0</v>
+      <c r="B3" s="11" t="n">
+        <v>42680.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="n">
-        <v>86.0</v>
+      <c r="B4" s="12" t="n">
+        <v>42687.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="n">
-        <v>81.0</v>
+      <c r="B5" s="13" t="n">
+        <v>42688.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="n">
-        <v>79.0</v>
+      <c r="B6" s="14" t="n">
+        <v>42694.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="n">
-        <v>73.0</v>
+      <c r="B7" s="15" t="n">
+        <v>42709.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="n">
-        <v>61.0</v>
+      <c r="B8" s="16" t="n">
+        <v>42709.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="n">
-        <v>68.0</v>
+      <c r="B9" s="17" t="n">
+        <v>42716.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="n">
-        <v>69.0</v>
+      <c r="B10" s="18" t="n">
+        <v>42717.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="n">
-        <v>72.0</v>
+      <c r="B11" s="19" t="n">
+        <v>42723.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="n">
-        <v>87.0</v>
+      <c r="B12" s="20" t="n">
+        <v>42723.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>